<commit_message>
new modified initial DoE
</commit_message>
<xml_diff>
--- a/DoE_csv/PhD_MasterDataset_OT_initial.xlsx
+++ b/DoE_csv/PhD_MasterDataset_OT_initial.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/DoE_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D10E3325-27B4-AD4C-908B-54B1F645F362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44773CE8-1A38-0141-96EF-F1D9C9824BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhD_MasterDataset_OT_initial" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>ID</t>
   </si>
@@ -212,13 +212,121 @@
   </si>
   <si>
     <t>S42</t>
+  </si>
+  <si>
+    <t>S43</t>
+  </si>
+  <si>
+    <t>S44</t>
+  </si>
+  <si>
+    <t>S45</t>
+  </si>
+  <si>
+    <t>S46</t>
+  </si>
+  <si>
+    <t>S47</t>
+  </si>
+  <si>
+    <t>S48</t>
+  </si>
+  <si>
+    <t>S49</t>
+  </si>
+  <si>
+    <t>S50</t>
+  </si>
+  <si>
+    <t>S51</t>
+  </si>
+  <si>
+    <t>S52</t>
+  </si>
+  <si>
+    <t>S53</t>
+  </si>
+  <si>
+    <t>S54</t>
+  </si>
+  <si>
+    <t>S55</t>
+  </si>
+  <si>
+    <t>S56</t>
+  </si>
+  <si>
+    <t>S57</t>
+  </si>
+  <si>
+    <t>S58</t>
+  </si>
+  <si>
+    <t>S59</t>
+  </si>
+  <si>
+    <t>S60</t>
+  </si>
+  <si>
+    <t>S61</t>
+  </si>
+  <si>
+    <t>S62</t>
+  </si>
+  <si>
+    <t>S63</t>
+  </si>
+  <si>
+    <t>S64</t>
+  </si>
+  <si>
+    <t>S65</t>
+  </si>
+  <si>
+    <t>S66</t>
+  </si>
+  <si>
+    <t>S67</t>
+  </si>
+  <si>
+    <t>S68</t>
+  </si>
+  <si>
+    <t>S69</t>
+  </si>
+  <si>
+    <t>S70</t>
+  </si>
+  <si>
+    <t>S71</t>
+  </si>
+  <si>
+    <t>S72</t>
+  </si>
+  <si>
+    <t>S73</t>
+  </si>
+  <si>
+    <t>S74</t>
+  </si>
+  <si>
+    <t>S75</t>
+  </si>
+  <si>
+    <t>S76</t>
+  </si>
+  <si>
+    <t>S77</t>
+  </si>
+  <si>
+    <t>S78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +460,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -695,8 +815,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1051,11 +1172,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:V43"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3640,6 +3761,9 @@
       <c r="U38">
         <v>69</v>
       </c>
+      <c r="V38">
+        <v>1.02</v>
+      </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -3705,6 +3829,9 @@
       <c r="U39">
         <v>69</v>
       </c>
+      <c r="V39">
+        <v>1.0169999999999999</v>
+      </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -3770,6 +3897,9 @@
       <c r="U40">
         <v>68</v>
       </c>
+      <c r="V40">
+        <v>1.0129999999999999</v>
+      </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -3835,6 +3965,9 @@
       <c r="U41">
         <v>80</v>
       </c>
+      <c r="V41">
+        <v>1.0089999999999999</v>
+      </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -3900,6 +4033,9 @@
       <c r="U42">
         <v>74</v>
       </c>
+      <c r="V42">
+        <v>1.006</v>
+      </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -3965,8 +4101,2244 @@
       <c r="U43">
         <v>68</v>
       </c>
+      <c r="V43">
+        <v>1.018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45" s="1">
+        <v>2</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45" s="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46" s="1">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C49" s="1">
+        <v>11</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50" s="1">
+        <v>2</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51" s="1">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+      <c r="T52" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>11.3</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+      <c r="T57" s="1">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+      <c r="T58" s="1">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+      <c r="T59" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>12</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60" s="1">
+        <v>3</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+      <c r="T61" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="M62" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+      <c r="T62" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63" s="1">
+        <v>11.3</v>
+      </c>
+      <c r="M63" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="M64" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <v>0</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="M65" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+      <c r="T65" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="M66" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67" s="1">
+        <v>10.8</v>
+      </c>
+      <c r="M67" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+      <c r="T67" s="1">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="O68" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+      <c r="T68" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>89</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="O69" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+      <c r="T69" s="1">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="O70" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0</v>
+      </c>
+      <c r="T70" s="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="O71" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="O72" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73" s="1">
+        <v>12</v>
+      </c>
+      <c r="O73" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
+        <v>0</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="S73">
+        <v>0</v>
+      </c>
+      <c r="T73" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>94</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" s="1">
+        <v>9</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+      <c r="T74" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>0</v>
+      </c>
+      <c r="T75" s="1">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>0</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>0</v>
+      </c>
+      <c r="T76" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>0</v>
+      </c>
+      <c r="O77" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>0</v>
+      </c>
+      <c r="T77" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>98</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>10.1</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>12.3</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+      <c r="T79" s="1">
+        <v>2.8</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change order of surfactant pairs in DoE
</commit_message>
<xml_diff>
--- a/DoE_csv/PhD_MasterDataset_OT_initial.xlsx
+++ b/DoE_csv/PhD_MasterDataset_OT_initial.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/DoE_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44773CE8-1A38-0141-96EF-F1D9C9824BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89013DAC-864B-304F-95F5-3CCFDC7C54CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200"/>
   </bookViews>
   <sheets>
-    <sheet name="PhD_MasterDataset_OT_initial" sheetId="1" r:id="rId1"/>
+    <sheet name="PhD_MasterDataset_OT_initial_Ja" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -325,8 +325,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -460,18 +460,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -815,9 +803,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1172,12 +1159,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="V44" sqref="V44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4112,7 +4097,7 @@
       <c r="B44" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
         <v>9.3000000000000007</v>
       </c>
       <c r="D44">
@@ -4133,7 +4118,7 @@
       <c r="I44">
         <v>0</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44">
         <v>10.5</v>
       </c>
       <c r="K44">
@@ -4148,7 +4133,7 @@
       <c r="N44">
         <v>0</v>
       </c>
-      <c r="O44" s="1">
+      <c r="O44">
         <v>1.3</v>
       </c>
       <c r="P44">
@@ -4163,8 +4148,14 @@
       <c r="S44">
         <v>0</v>
       </c>
-      <c r="T44" s="1">
+      <c r="T44">
         <v>3.2</v>
+      </c>
+      <c r="U44">
+        <v>75.7</v>
+      </c>
+      <c r="V44">
+        <v>1.018</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -4174,7 +4165,7 @@
       <c r="B45" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>8.6999999999999993</v>
       </c>
       <c r="D45">
@@ -4195,7 +4186,7 @@
       <c r="I45">
         <v>0</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45">
         <v>8.1999999999999993</v>
       </c>
       <c r="K45">
@@ -4210,7 +4201,7 @@
       <c r="N45">
         <v>0</v>
       </c>
-      <c r="O45" s="1">
+      <c r="O45">
         <v>2</v>
       </c>
       <c r="P45">
@@ -4225,8 +4216,14 @@
       <c r="S45">
         <v>0</v>
       </c>
-      <c r="T45" s="1">
+      <c r="T45">
         <v>3.6</v>
+      </c>
+      <c r="U45">
+        <v>77.5</v>
+      </c>
+      <c r="V45">
+        <v>1.016</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -4236,7 +4233,7 @@
       <c r="B46" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46">
         <v>12.3</v>
       </c>
       <c r="D46">
@@ -4257,7 +4254,7 @@
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46">
         <v>10.3</v>
       </c>
       <c r="K46">
@@ -4272,7 +4269,7 @@
       <c r="N46">
         <v>0</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O46">
         <v>1</v>
       </c>
       <c r="P46">
@@ -4287,8 +4284,14 @@
       <c r="S46">
         <v>0</v>
       </c>
-      <c r="T46" s="1">
+      <c r="T46">
         <v>1.9</v>
+      </c>
+      <c r="U46">
+        <v>74.5</v>
+      </c>
+      <c r="V46">
+        <v>1.0209999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -4298,7 +4301,7 @@
       <c r="B47" t="s">
         <v>67</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>12.5</v>
       </c>
       <c r="D47">
@@ -4319,7 +4322,7 @@
       <c r="I47">
         <v>0</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47">
         <v>12.8</v>
       </c>
       <c r="K47">
@@ -4334,7 +4337,7 @@
       <c r="N47">
         <v>0</v>
       </c>
-      <c r="O47" s="1">
+      <c r="O47">
         <v>1.6</v>
       </c>
       <c r="P47">
@@ -4349,8 +4352,14 @@
       <c r="S47">
         <v>0</v>
       </c>
-      <c r="T47" s="1">
+      <c r="T47">
         <v>4.5</v>
+      </c>
+      <c r="U47">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="V47">
+        <v>1.024</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -4360,7 +4369,7 @@
       <c r="B48" t="s">
         <v>68</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
         <v>9.9</v>
       </c>
       <c r="D48">
@@ -4381,7 +4390,7 @@
       <c r="I48">
         <v>0</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48">
         <v>9.4</v>
       </c>
       <c r="K48">
@@ -4396,7 +4405,7 @@
       <c r="N48">
         <v>0</v>
       </c>
-      <c r="O48" s="1">
+      <c r="O48">
         <v>1.3</v>
       </c>
       <c r="P48">
@@ -4411,18 +4420,24 @@
       <c r="S48">
         <v>0</v>
       </c>
-      <c r="T48" s="1">
+      <c r="T48">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U48">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="V48">
+        <v>1.018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
         <v>11</v>
       </c>
       <c r="D49">
@@ -4443,7 +4458,7 @@
       <c r="I49">
         <v>0</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49">
         <v>8.3000000000000007</v>
       </c>
       <c r="K49">
@@ -4458,7 +4473,7 @@
       <c r="N49">
         <v>0</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O49">
         <v>1.7</v>
       </c>
       <c r="P49">
@@ -4473,11 +4488,17 @@
       <c r="S49">
         <v>0</v>
       </c>
-      <c r="T49" s="1">
+      <c r="T49">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U49">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="V49">
+        <v>1.018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4487,20 +4508,20 @@
       <c r="C50">
         <v>0</v>
       </c>
-      <c r="D50" s="1">
-        <v>12.1</v>
+      <c r="D50">
+        <v>0</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>12.8</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
-      <c r="H50" s="1">
-        <v>12.3</v>
+      <c r="H50">
+        <v>0</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -4518,10 +4539,10 @@
         <v>0</v>
       </c>
       <c r="N50">
-        <v>0</v>
-      </c>
-      <c r="O50" s="1">
-        <v>2</v>
+        <v>9.5</v>
+      </c>
+      <c r="O50">
+        <v>1.9</v>
       </c>
       <c r="P50">
         <v>0</v>
@@ -4535,11 +4556,17 @@
       <c r="S50">
         <v>0</v>
       </c>
-      <c r="T50" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T50">
+        <v>3</v>
+      </c>
+      <c r="U50">
+        <v>72.8</v>
+      </c>
+      <c r="V50">
+        <v>1.0069999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4549,20 +4576,20 @@
       <c r="C51">
         <v>0</v>
       </c>
-      <c r="D51" s="1">
-        <v>12.9</v>
+      <c r="D51">
+        <v>0</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>11.2</v>
       </c>
       <c r="G51">
         <v>0</v>
       </c>
-      <c r="H51" s="1">
-        <v>9.6999999999999993</v>
+      <c r="H51">
+        <v>0</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -4580,10 +4607,10 @@
         <v>0</v>
       </c>
       <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="O51" s="1">
-        <v>2.2000000000000002</v>
+        <v>11.8</v>
+      </c>
+      <c r="O51">
+        <v>2.8</v>
       </c>
       <c r="P51">
         <v>0</v>
@@ -4597,11 +4624,17 @@
       <c r="S51">
         <v>0</v>
       </c>
-      <c r="T51" s="1">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T51">
+        <v>2.6</v>
+      </c>
+      <c r="U51">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="V51">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4611,20 +4644,20 @@
       <c r="C52">
         <v>0</v>
       </c>
-      <c r="D52" s="1">
-        <v>8.9</v>
+      <c r="D52">
+        <v>0</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>9.4</v>
       </c>
       <c r="G52">
         <v>0</v>
       </c>
-      <c r="H52" s="1">
-        <v>12.5</v>
+      <c r="H52">
+        <v>0</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -4642,10 +4675,10 @@
         <v>0</v>
       </c>
       <c r="N52">
-        <v>0</v>
-      </c>
-      <c r="O52" s="1">
-        <v>1.4</v>
+        <v>11.7</v>
+      </c>
+      <c r="O52">
+        <v>1.8</v>
       </c>
       <c r="P52">
         <v>0</v>
@@ -4659,11 +4692,17 @@
       <c r="S52">
         <v>0</v>
       </c>
-      <c r="T52" s="1">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T52">
+        <v>3.3</v>
+      </c>
+      <c r="U52">
+        <v>73.8</v>
+      </c>
+      <c r="V52">
+        <v>1.0029999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4673,20 +4712,20 @@
       <c r="C53">
         <v>0</v>
       </c>
-      <c r="D53" s="1">
-        <v>11.3</v>
+      <c r="D53">
+        <v>0</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
-      <c r="H53" s="1">
-        <v>9.9</v>
+      <c r="H53">
+        <v>0</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -4704,10 +4743,10 @@
         <v>0</v>
       </c>
       <c r="N53">
-        <v>0</v>
-      </c>
-      <c r="O53" s="1">
-        <v>1.5</v>
+        <v>11.1</v>
+      </c>
+      <c r="O53">
+        <v>2.4</v>
       </c>
       <c r="P53">
         <v>0</v>
@@ -4721,11 +4760,17 @@
       <c r="S53">
         <v>0</v>
       </c>
-      <c r="T53" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T53">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="U53">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="V53">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4735,20 +4780,20 @@
       <c r="C54">
         <v>0</v>
       </c>
-      <c r="D54" s="1">
-        <v>10.1</v>
+      <c r="D54">
+        <v>0</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="G54">
         <v>0</v>
       </c>
-      <c r="H54" s="1">
-        <v>12.9</v>
+      <c r="H54">
+        <v>0</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -4766,10 +4811,10 @@
         <v>0</v>
       </c>
       <c r="N54">
-        <v>0</v>
-      </c>
-      <c r="O54" s="1">
-        <v>2.5</v>
+        <v>8.1</v>
+      </c>
+      <c r="O54">
+        <v>1.8</v>
       </c>
       <c r="P54">
         <v>0</v>
@@ -4783,11 +4828,17 @@
       <c r="S54">
         <v>0</v>
       </c>
-      <c r="T54" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T54">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U54">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="V54">
+        <v>1.006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4797,20 +4848,20 @@
       <c r="C55">
         <v>0</v>
       </c>
-      <c r="D55" s="1">
-        <v>8.6999999999999993</v>
+      <c r="D55">
+        <v>0</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>11.7</v>
       </c>
       <c r="G55">
         <v>0</v>
       </c>
-      <c r="H55" s="1">
-        <v>12.4</v>
+      <c r="H55">
+        <v>0</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -4828,10 +4879,10 @@
         <v>0</v>
       </c>
       <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="O55" s="1">
-        <v>2.8</v>
+        <v>12</v>
+      </c>
+      <c r="O55">
+        <v>2.2999999999999998</v>
       </c>
       <c r="P55">
         <v>0</v>
@@ -4845,11 +4896,17 @@
       <c r="S55">
         <v>0</v>
       </c>
-      <c r="T55" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T55">
+        <v>3.4</v>
+      </c>
+      <c r="U55">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="V55">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4862,26 +4919,26 @@
       <c r="D56">
         <v>0</v>
       </c>
-      <c r="E56" s="1">
-        <v>9.6999999999999993</v>
+      <c r="E56">
+        <v>0</v>
       </c>
       <c r="F56">
         <v>0</v>
       </c>
-      <c r="G56" s="1">
-        <v>12.7</v>
+      <c r="G56">
+        <v>0</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J56">
         <v>0</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -4892,8 +4949,8 @@
       <c r="N56">
         <v>0</v>
       </c>
-      <c r="O56" s="1">
-        <v>2.1</v>
+      <c r="O56">
+        <v>1.8</v>
       </c>
       <c r="P56">
         <v>0</v>
@@ -4907,11 +4964,17 @@
       <c r="S56">
         <v>0</v>
       </c>
-      <c r="T56" s="1">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T56">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="U56">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="V56">
+        <v>1.0069999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4924,26 +4987,26 @@
       <c r="D57">
         <v>0</v>
       </c>
-      <c r="E57" s="1">
-        <v>10.6</v>
+      <c r="E57">
+        <v>0</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
-      <c r="G57" s="1">
-        <v>10.4</v>
+      <c r="G57">
+        <v>0</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>11.6</v>
       </c>
       <c r="J57">
         <v>0</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="L57">
         <v>0</v>
@@ -4954,8 +5017,8 @@
       <c r="N57">
         <v>0</v>
       </c>
-      <c r="O57" s="1">
-        <v>2.6</v>
+      <c r="O57">
+        <v>2.4</v>
       </c>
       <c r="P57">
         <v>0</v>
@@ -4969,11 +5032,17 @@
       <c r="S57">
         <v>0</v>
       </c>
-      <c r="T57" s="1">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T57">
+        <v>1.6</v>
+      </c>
+      <c r="U57">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="V57">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4986,26 +5055,26 @@
       <c r="D58">
         <v>0</v>
       </c>
-      <c r="E58" s="1">
-        <v>11.4</v>
+      <c r="E58">
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0</v>
       </c>
-      <c r="G58" s="1">
-        <v>11.4</v>
+      <c r="G58">
+        <v>0</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>10.9</v>
       </c>
       <c r="J58">
         <v>0</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>10.7</v>
       </c>
       <c r="L58">
         <v>0</v>
@@ -5016,8 +5085,8 @@
       <c r="N58">
         <v>0</v>
       </c>
-      <c r="O58" s="1">
-        <v>1.2</v>
+      <c r="O58">
+        <v>2.5</v>
       </c>
       <c r="P58">
         <v>0</v>
@@ -5031,11 +5100,17 @@
       <c r="S58">
         <v>0</v>
       </c>
-      <c r="T58" s="1">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T58">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U58">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="V58">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5048,26 +5123,26 @@
       <c r="D59">
         <v>0</v>
       </c>
-      <c r="E59" s="1">
-        <v>9.1999999999999993</v>
+      <c r="E59">
+        <v>0</v>
       </c>
       <c r="F59">
         <v>0</v>
       </c>
-      <c r="G59" s="1">
-        <v>9.1</v>
+      <c r="G59">
+        <v>0</v>
       </c>
       <c r="H59">
         <v>0</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>12.7</v>
       </c>
       <c r="J59">
         <v>0</v>
       </c>
       <c r="K59">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -5078,8 +5153,8 @@
       <c r="N59">
         <v>0</v>
       </c>
-      <c r="O59" s="1">
-        <v>2.2999999999999998</v>
+      <c r="O59">
+        <v>2.7</v>
       </c>
       <c r="P59">
         <v>0</v>
@@ -5093,11 +5168,17 @@
       <c r="S59">
         <v>0</v>
       </c>
-      <c r="T59" s="1">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T59">
+        <v>1.3</v>
+      </c>
+      <c r="U59">
+        <v>71.8</v>
+      </c>
+      <c r="V59">
+        <v>1.012</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -5110,26 +5191,26 @@
       <c r="D60">
         <v>0</v>
       </c>
-      <c r="E60" s="1">
-        <v>12</v>
+      <c r="E60">
+        <v>0</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
-      <c r="G60" s="1">
-        <v>9.1999999999999993</v>
+      <c r="G60">
+        <v>0</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>10.1</v>
       </c>
       <c r="J60">
         <v>0</v>
       </c>
       <c r="K60">
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -5140,8 +5221,8 @@
       <c r="N60">
         <v>0</v>
       </c>
-      <c r="O60" s="1">
-        <v>3</v>
+      <c r="O60">
+        <v>2.9</v>
       </c>
       <c r="P60">
         <v>0</v>
@@ -5155,11 +5236,17 @@
       <c r="S60">
         <v>0</v>
       </c>
-      <c r="T60" s="1">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T60">
+        <v>2</v>
+      </c>
+      <c r="U60">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="V60">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -5172,26 +5259,26 @@
       <c r="D61">
         <v>0</v>
       </c>
-      <c r="E61" s="1">
-        <v>9.5</v>
+      <c r="E61">
+        <v>0</v>
       </c>
       <c r="F61">
         <v>0</v>
       </c>
-      <c r="G61" s="1">
-        <v>8.8000000000000007</v>
+      <c r="G61">
+        <v>0</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="J61">
         <v>0</v>
       </c>
       <c r="K61">
-        <v>0</v>
+        <v>8.6</v>
       </c>
       <c r="L61">
         <v>0</v>
@@ -5202,8 +5289,8 @@
       <c r="N61">
         <v>0</v>
       </c>
-      <c r="O61" s="1">
-        <v>2.7</v>
+      <c r="O61">
+        <v>1.5</v>
       </c>
       <c r="P61">
         <v>0</v>
@@ -5217,11 +5304,17 @@
       <c r="S61">
         <v>0</v>
       </c>
-      <c r="T61" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T61">
+        <v>2.8</v>
+      </c>
+      <c r="U61">
+        <v>74.8</v>
+      </c>
+      <c r="V61">
+        <v>1.0089999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -5255,16 +5348,16 @@
       <c r="K62">
         <v>0</v>
       </c>
-      <c r="L62" s="1">
+      <c r="L62">
         <v>8.9</v>
       </c>
-      <c r="M62" s="1">
+      <c r="M62">
         <v>8.4</v>
       </c>
       <c r="N62">
         <v>0</v>
       </c>
-      <c r="O62" s="1">
+      <c r="O62">
         <v>1.1000000000000001</v>
       </c>
       <c r="P62">
@@ -5279,11 +5372,17 @@
       <c r="S62">
         <v>0</v>
       </c>
-      <c r="T62" s="1">
+      <c r="T62">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U62">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="V62">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -5317,16 +5416,16 @@
       <c r="K63">
         <v>0</v>
       </c>
-      <c r="L63" s="1">
+      <c r="L63">
         <v>11.3</v>
       </c>
-      <c r="M63" s="1">
+      <c r="M63">
         <v>10.199999999999999</v>
       </c>
       <c r="N63">
         <v>0</v>
       </c>
-      <c r="O63" s="1">
+      <c r="O63">
         <v>1.2</v>
       </c>
       <c r="P63">
@@ -5341,11 +5440,17 @@
       <c r="S63">
         <v>0</v>
       </c>
-      <c r="T63" s="1">
+      <c r="T63">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U63">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="V63">
+        <v>1.0069999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -5379,16 +5484,16 @@
       <c r="K64">
         <v>0</v>
       </c>
-      <c r="L64" s="1">
+      <c r="L64">
         <v>10.9</v>
       </c>
-      <c r="M64" s="1">
+      <c r="M64">
         <v>8.3000000000000007</v>
       </c>
       <c r="N64">
         <v>0</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O64">
         <v>1.6</v>
       </c>
       <c r="P64">
@@ -5403,11 +5508,17 @@
       <c r="S64">
         <v>0</v>
       </c>
-      <c r="T64" s="1">
+      <c r="T64">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U64">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="V64">
+        <v>1.0069999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -5441,16 +5552,16 @@
       <c r="K65">
         <v>0</v>
       </c>
-      <c r="L65" s="1">
+      <c r="L65">
         <v>11.9</v>
       </c>
-      <c r="M65" s="1">
+      <c r="M65">
         <v>10.5</v>
       </c>
       <c r="N65">
         <v>0</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O65">
         <v>1.1000000000000001</v>
       </c>
       <c r="P65">
@@ -5465,11 +5576,17 @@
       <c r="S65">
         <v>0</v>
       </c>
-      <c r="T65" s="1">
+      <c r="T65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U65">
+        <v>72.5</v>
+      </c>
+      <c r="V65">
+        <v>1.0069999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -5503,16 +5620,16 @@
       <c r="K66">
         <v>0</v>
       </c>
-      <c r="L66" s="1">
+      <c r="L66">
         <v>10.1</v>
       </c>
-      <c r="M66" s="1">
+      <c r="M66">
         <v>8.1</v>
       </c>
       <c r="N66">
         <v>0</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O66">
         <v>2.6</v>
       </c>
       <c r="P66">
@@ -5527,11 +5644,17 @@
       <c r="S66">
         <v>0</v>
       </c>
-      <c r="T66" s="1">
+      <c r="T66">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U66">
+        <v>76.7</v>
+      </c>
+      <c r="V66">
+        <v>1.008</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -5565,16 +5688,16 @@
       <c r="K67">
         <v>0</v>
       </c>
-      <c r="L67" s="1">
+      <c r="L67">
         <v>10.8</v>
       </c>
-      <c r="M67" s="1">
+      <c r="M67">
         <v>11.8</v>
       </c>
       <c r="N67">
         <v>0</v>
       </c>
-      <c r="O67" s="1">
+      <c r="O67">
         <v>2.2000000000000002</v>
       </c>
       <c r="P67">
@@ -5589,11 +5712,17 @@
       <c r="S67">
         <v>0</v>
       </c>
-      <c r="T67" s="1">
+      <c r="T67">
         <v>3.7</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U67">
+        <v>71.5</v>
+      </c>
+      <c r="V67">
+        <v>1.008</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -5604,19 +5733,19 @@
         <v>0</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
-      <c r="F68" s="1">
-        <v>12.8</v>
+      <c r="F68">
+        <v>0</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="I68">
         <v>0</v>
@@ -5633,11 +5762,11 @@
       <c r="M68">
         <v>0</v>
       </c>
-      <c r="N68" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="O68" s="1">
-        <v>1.9</v>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>2</v>
       </c>
       <c r="P68">
         <v>0</v>
@@ -5651,11 +5780,17 @@
       <c r="S68">
         <v>0</v>
       </c>
-      <c r="T68" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T68">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U68">
+        <v>71.3</v>
+      </c>
+      <c r="V68">
+        <v>1.0269999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -5666,19 +5801,19 @@
         <v>0</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69" s="1">
-        <v>11.2</v>
+      <c r="F69">
+        <v>0</v>
       </c>
       <c r="G69">
         <v>0</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -5695,11 +5830,11 @@
       <c r="M69">
         <v>0</v>
       </c>
-      <c r="N69" s="1">
-        <v>11.8</v>
-      </c>
-      <c r="O69" s="1">
-        <v>2.8</v>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>2.2000000000000002</v>
       </c>
       <c r="P69">
         <v>0</v>
@@ -5713,11 +5848,17 @@
       <c r="S69">
         <v>0</v>
       </c>
-      <c r="T69" s="1">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T69">
+        <v>4.3</v>
+      </c>
+      <c r="U69">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="V69">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -5728,19 +5869,19 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="F70" s="1">
-        <v>9.4</v>
+      <c r="F70">
+        <v>0</v>
       </c>
       <c r="G70">
         <v>0</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -5757,11 +5898,11 @@
       <c r="M70">
         <v>0</v>
       </c>
-      <c r="N70" s="1">
-        <v>11.7</v>
-      </c>
-      <c r="O70" s="1">
-        <v>1.8</v>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>1.4</v>
       </c>
       <c r="P70">
         <v>0</v>
@@ -5775,11 +5916,17 @@
       <c r="S70">
         <v>0</v>
       </c>
-      <c r="T70" s="1">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T70">
+        <v>1.4</v>
+      </c>
+      <c r="U70">
+        <v>75.8</v>
+      </c>
+      <c r="V70">
+        <v>1.022</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -5790,19 +5937,19 @@
         <v>0</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>11.3</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71" s="1">
-        <v>8.3000000000000007</v>
+      <c r="F71">
+        <v>0</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>9.9</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -5819,11 +5966,11 @@
       <c r="M71">
         <v>0</v>
       </c>
-      <c r="N71" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="O71" s="1">
-        <v>2.4</v>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>1.5</v>
       </c>
       <c r="P71">
         <v>0</v>
@@ -5837,11 +5984,17 @@
       <c r="S71">
         <v>0</v>
       </c>
-      <c r="T71" s="1">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T71">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U71">
+        <v>76.2</v>
+      </c>
+      <c r="V71">
+        <v>1.0229999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -5852,19 +6005,19 @@
         <v>0</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>10.1</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72" s="1">
-        <v>10.4</v>
+      <c r="F72">
+        <v>0</v>
       </c>
       <c r="G72">
         <v>0</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -5881,11 +6034,11 @@
       <c r="M72">
         <v>0</v>
       </c>
-      <c r="N72" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="O72" s="1">
-        <v>1.8</v>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>2.5</v>
       </c>
       <c r="P72">
         <v>0</v>
@@ -5899,11 +6052,17 @@
       <c r="S72">
         <v>0</v>
       </c>
-      <c r="T72" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T72">
+        <v>3</v>
+      </c>
+      <c r="U72">
+        <v>71.5</v>
+      </c>
+      <c r="V72">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -5914,19 +6073,19 @@
         <v>0</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73" s="1">
-        <v>11.7</v>
+      <c r="F73">
+        <v>0</v>
       </c>
       <c r="G73">
         <v>0</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>12.4</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -5943,11 +6102,11 @@
       <c r="M73">
         <v>0</v>
       </c>
-      <c r="N73" s="1">
-        <v>12</v>
-      </c>
-      <c r="O73" s="1">
-        <v>2.2999999999999998</v>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>2.8</v>
       </c>
       <c r="P73">
         <v>0</v>
@@ -5961,11 +6120,17 @@
       <c r="S73">
         <v>0</v>
       </c>
-      <c r="T73" s="1">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T73">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="U73">
+        <v>72</v>
+      </c>
+      <c r="V73">
+        <v>1.0229999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5979,25 +6144,25 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="F74">
         <v>0</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>12.7</v>
       </c>
       <c r="H74">
         <v>0</v>
       </c>
-      <c r="I74" s="1">
-        <v>9</v>
+      <c r="I74">
+        <v>0</v>
       </c>
       <c r="J74">
         <v>0</v>
       </c>
-      <c r="K74" s="1">
-        <v>10.199999999999999</v>
+      <c r="K74">
+        <v>0</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -6008,8 +6173,8 @@
       <c r="N74">
         <v>0</v>
       </c>
-      <c r="O74" s="1">
-        <v>1.8</v>
+      <c r="O74">
+        <v>2.1</v>
       </c>
       <c r="P74">
         <v>0</v>
@@ -6023,11 +6188,17 @@
       <c r="S74">
         <v>0</v>
       </c>
-      <c r="T74" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T74">
+        <v>1.9</v>
+      </c>
+      <c r="U74">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="V74">
+        <v>1.0189999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6041,25 +6212,25 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>10.6</v>
       </c>
       <c r="F75">
         <v>0</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="H75">
         <v>0</v>
       </c>
-      <c r="I75" s="1">
-        <v>11.6</v>
+      <c r="I75">
+        <v>0</v>
       </c>
       <c r="J75">
         <v>0</v>
       </c>
-      <c r="K75" s="1">
-        <v>8.5</v>
+      <c r="K75">
+        <v>0</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -6070,8 +6241,8 @@
       <c r="N75">
         <v>0</v>
       </c>
-      <c r="O75" s="1">
-        <v>2.4</v>
+      <c r="O75">
+        <v>2.6</v>
       </c>
       <c r="P75">
         <v>0</v>
@@ -6085,11 +6256,17 @@
       <c r="S75">
         <v>0</v>
       </c>
-      <c r="T75" s="1">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T75">
+        <v>4.2</v>
+      </c>
+      <c r="U75">
+        <v>72.2</v>
+      </c>
+      <c r="V75">
+        <v>1.0169999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6103,25 +6280,25 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>11.4</v>
       </c>
       <c r="F76">
         <v>0</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>11.4</v>
       </c>
       <c r="H76">
         <v>0</v>
       </c>
-      <c r="I76" s="1">
-        <v>10.9</v>
+      <c r="I76">
+        <v>0</v>
       </c>
       <c r="J76">
         <v>0</v>
       </c>
-      <c r="K76" s="1">
-        <v>10.7</v>
+      <c r="K76">
+        <v>0</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -6132,8 +6309,8 @@
       <c r="N76">
         <v>0</v>
       </c>
-      <c r="O76" s="1">
-        <v>2.5</v>
+      <c r="O76">
+        <v>1.2</v>
       </c>
       <c r="P76">
         <v>0</v>
@@ -6147,11 +6324,17 @@
       <c r="S76">
         <v>0</v>
       </c>
-      <c r="T76" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T76">
+        <v>4.7</v>
+      </c>
+      <c r="U76">
+        <v>71.3</v>
+      </c>
+      <c r="V76">
+        <v>1.0169999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6165,25 +6348,25 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F77">
         <v>0</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="H77">
         <v>0</v>
       </c>
-      <c r="I77" s="1">
-        <v>12.7</v>
+      <c r="I77">
+        <v>0</v>
       </c>
       <c r="J77">
         <v>0</v>
       </c>
-      <c r="K77" s="1">
-        <v>11.5</v>
+      <c r="K77">
+        <v>0</v>
       </c>
       <c r="L77">
         <v>0</v>
@@ -6194,8 +6377,8 @@
       <c r="N77">
         <v>0</v>
       </c>
-      <c r="O77" s="1">
-        <v>2.7</v>
+      <c r="O77">
+        <v>2.2999999999999998</v>
       </c>
       <c r="P77">
         <v>0</v>
@@ -6209,11 +6392,17 @@
       <c r="S77">
         <v>0</v>
       </c>
-      <c r="T77" s="1">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T77">
+        <v>1.5</v>
+      </c>
+      <c r="U77">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="V77">
+        <v>1.0149999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6227,25 +6416,25 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H78">
         <v>0</v>
       </c>
-      <c r="I78" s="1">
-        <v>10.1</v>
+      <c r="I78">
+        <v>0</v>
       </c>
       <c r="J78">
         <v>0</v>
       </c>
-      <c r="K78" s="1">
-        <v>9.6</v>
+      <c r="K78">
+        <v>0</v>
       </c>
       <c r="L78">
         <v>0</v>
@@ -6256,8 +6445,8 @@
       <c r="N78">
         <v>0</v>
       </c>
-      <c r="O78" s="1">
-        <v>2.9</v>
+      <c r="O78">
+        <v>3</v>
       </c>
       <c r="P78">
         <v>0</v>
@@ -6271,11 +6460,17 @@
       <c r="S78">
         <v>0</v>
       </c>
-      <c r="T78" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T78">
+        <v>3.5</v>
+      </c>
+      <c r="U78">
+        <v>72.3</v>
+      </c>
+      <c r="V78">
+        <v>1.0169999999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6289,25 +6484,25 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="F79">
         <v>0</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
-      <c r="I79" s="1">
-        <v>12.3</v>
+      <c r="I79">
+        <v>0</v>
       </c>
       <c r="J79">
         <v>0</v>
       </c>
-      <c r="K79" s="1">
-        <v>8.6</v>
+      <c r="K79">
+        <v>0</v>
       </c>
       <c r="L79">
         <v>0</v>
@@ -6318,8 +6513,8 @@
       <c r="N79">
         <v>0</v>
       </c>
-      <c r="O79" s="1">
-        <v>1.5</v>
+      <c r="O79">
+        <v>2.7</v>
       </c>
       <c r="P79">
         <v>0</v>
@@ -6333,12 +6528,17 @@
       <c r="S79">
         <v>0</v>
       </c>
-      <c r="T79" s="1">
-        <v>2.8</v>
+      <c r="T79">
+        <v>5</v>
+      </c>
+      <c r="U79">
+        <v>74</v>
+      </c>
+      <c r="V79">
+        <v>1.014</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>